<commit_message>
modifikovana tabulka pre lepsiu citatelnost
</commit_message>
<xml_diff>
--- a/tabluka1.xlsx
+++ b/tabluka1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonukus/Desktop/MIP_clanok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458465A9-9282-C342-8EE7-E671F0910FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFB23C1-2BC1-AF4D-AFEC-EE52F5DDB76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F35AEC75-9237-9A42-BC7C-42D4FFACAE1A}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,6 +146,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,10 +287,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -311,17 +320,143 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -348,6 +483,32 @@
         <right style="thin">
           <color auto="1"/>
         </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top/>
         <bottom/>
         <vertical style="thin">
@@ -357,154 +518,6 @@
           <color auto="1"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -520,16 +533,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCC3FD8E-44E3-DA40-AAB8-F03147CA1645}" name="Table1" displayName="Table1" ref="A1:E9" headerRowDxfId="1" dataDxfId="13" totalsRowDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
-  <autoFilter ref="A1:E9" xr:uid="{BCC3FD8E-44E3-DA40-AAB8-F03147CA1645}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BCC3FD8E-44E3-DA40-AAB8-F03147CA1645}" name="Table1" displayName="Table1" ref="A1:E9" headerRowDxfId="13" dataDxfId="11" totalsRowDxfId="9" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="A1:E9" xr:uid="{BCC3FD8E-44E3-DA40-AAB8-F03147CA1645}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A2837CBE-8327-5F47-9473-9FA04D6C7388}" name="č." totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{6029F270-45EA-C146-AD41-B071961B225A}" name="nástroj CASE" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{7BB8F1BE-47ED-FE4D-9D35-3ED232A356B9}" name="informácie" dataDxfId="4" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{C95BCB30-5489-7C47-B4AD-B9488EFCD2CF}" name="Predajca" dataDxfId="3" totalsRowDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{E6E1FCC9-386B-9443-84BD-B395E4D90155}" name="Typ Licencie" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{A2837CBE-8327-5F47-9473-9FA04D6C7388}" name="č." totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6029F270-45EA-C146-AD41-B071961B225A}" name="nástroj CASE" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7BB8F1BE-47ED-FE4D-9D35-3ED232A356B9}" name="informácie" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C95BCB30-5489-7C47-B4AD-B9488EFCD2CF}" name="Predajca" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E6E1FCC9-386B-9443-84BD-B395E4D90155}" name="Typ Licencie" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -833,7 +852,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,7 +886,7 @@
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -884,7 +903,7 @@
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -901,7 +920,7 @@
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -918,7 +937,7 @@
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -935,7 +954,7 @@
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -952,7 +971,7 @@
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="13" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -969,7 +988,7 @@
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -986,13 +1005,13 @@
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>